<commit_message>
Intermediate commit for making photo
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/Countries.xlsx
+++ b/DatabaseUpdate/ExcelFiles/Countries.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -22,6 +22,9 @@
     <x:t>Name</x:t>
   </x:si>
   <x:si>
+    <x:t>IsDefaultNationality</x:t>
+  </x:si>
+  <x:si>
     <x:t>BeginDateTime</x:t>
   </x:si>
   <x:si>
@@ -34,10 +37,16 @@
     <x:t>Российская Федерация</x:t>
   </x:si>
   <x:si>
+    <x:t>True</x:t>
+  </x:si>
+  <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>Казахстан</x:t>
+  </x:si>
+  <x:si>
+    <x:t>False</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -395,13 +404,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D3"/>
+  <x:dimension ref="A1:E3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -414,32 +423,41 @@
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="1">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D2" s="1">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D2" s="1">
+      <x:c r="E2" s="1">
         <x:v>2958465</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C3" s="1">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="1">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D3" s="1">
+      <x:c r="E3" s="1">
         <x:v>2958465</x:v>
       </x:c>
     </x:row>

</xml_diff>